<commit_message>
paper and supp figures
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carrie Zhu\Documents\Research\GWAS-frontera\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6253A0B3-EB76-4024-A3EA-84534769885C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A270986-C8CD-42CA-B931-CBBFFB1F97F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{F530DB7C-5B3A-4D87-B710-1F59E709F530}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{F530DB7C-5B3A-4D87-B710-1F59E709F530}"/>
   </bookViews>
   <sheets>
     <sheet name="phenotypes" sheetId="12" r:id="rId1"/>
@@ -33,6 +33,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'PGS (4)'!$A$3:$N$84</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'PGS (5)'!$A$3:$N$84</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">PGS_ave!$A$3:$N$84</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">phenotypes!$A$1:$E$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1614" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1615" uniqueCount="107">
   <si>
     <t>Phenotype</t>
   </si>
@@ -372,6 +373,9 @@
   <si>
     <t>female N</t>
   </si>
+  <si>
+    <t>sex diff ldsc</t>
+  </si>
 </sst>
 </file>
 
@@ -620,7 +624,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -665,6 +669,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -16558,10 +16563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E1A7214-04C0-41AD-9983-1B492084134C}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16571,19 +16576,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>105</v>
       </c>
     </row>
@@ -16592,7 +16597,7 @@
         <v>80</v>
       </c>
       <c r="C2">
-        <f>SUM(D2:E2)</f>
+        <f t="shared" ref="C2:C28" si="0">SUM(D2:E2)</f>
         <v>294338</v>
       </c>
       <c r="D2">
@@ -16607,7 +16612,7 @@
         <v>81</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C28" si="0">SUM(D3:E3)</f>
+        <f t="shared" si="0"/>
         <v>331074</v>
       </c>
       <c r="D3">
@@ -16637,7 +16642,7 @@
         <v>62</v>
       </c>
       <c r="C5">
-        <f>SUM(D5:E5)</f>
+        <f t="shared" si="0"/>
         <v>336020</v>
       </c>
       <c r="D5">
@@ -16992,8 +16997,16 @@
         <v>180420</v>
       </c>
     </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:E1" xr:uid="{0E1A7214-04C0-41AD-9983-1B492084134C}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -17027,24 +17040,24 @@
     <row r="2" spans="1:14" ht="26" x14ac:dyDescent="0.6">
       <c r="A2" s="6"/>
       <c r="B2" s="7"/>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="36" t="s">
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="36" t="s">
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
     </row>
     <row r="3" spans="1:14" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="15" t="s">
@@ -21408,24 +21421,24 @@
     <row r="2" spans="1:14" ht="26" x14ac:dyDescent="0.6">
       <c r="A2" s="6"/>
       <c r="B2" s="7"/>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="36" t="s">
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="36" t="s">
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
     </row>
     <row r="3" spans="1:14" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="15" t="s">
@@ -28484,8 +28497,8 @@
   <dimension ref="A1:H84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F52" sqref="F52"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -28578,19 +28591,19 @@
         <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
         <v>33</v>
       </c>
       <c r="D6">
-        <v>0.10630000000000001</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="E6">
-        <v>6.8999999999999999E-3</v>
+        <v>1.1299999999999999E-2</v>
       </c>
       <c r="F6">
-        <v>0.98</v>
+        <v>1.12E-2</v>
       </c>
       <c r="G6">
         <v>8.2000000000000007E-3</v>
@@ -28647,19 +28660,19 @@
         <v>30850</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
         <v>33</v>
       </c>
       <c r="D9">
-        <v>0.1973</v>
+        <v>0.12820000000000001</v>
       </c>
       <c r="E9">
-        <v>7.7000000000000002E-3</v>
+        <v>7.1999999999999998E-3</v>
       </c>
       <c r="F9">
-        <v>0.9728</v>
+        <v>0.63219999999999998</v>
       </c>
       <c r="G9">
         <v>5.21E-2</v>
@@ -28670,19 +28683,19 @@
         <v>21001</v>
       </c>
       <c r="B10" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
         <v>33</v>
       </c>
       <c r="D10">
-        <v>0.42020000000000002</v>
+        <v>0.158</v>
       </c>
       <c r="E10">
-        <v>1.7399999999999999E-2</v>
+        <v>5.3E-3</v>
       </c>
       <c r="F10">
-        <v>0.97230000000000005</v>
+        <v>0.75170000000000003</v>
       </c>
       <c r="G10">
         <v>1.37E-2</v>
@@ -28785,19 +28798,19 @@
         <v>30010</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s">
         <v>33</v>
       </c>
       <c r="D15">
-        <v>0.1065</v>
+        <v>0.157</v>
       </c>
       <c r="E15">
-        <v>1.11E-2</v>
+        <v>2.69E-2</v>
       </c>
       <c r="F15">
-        <v>0.96630000000000005</v>
+        <v>0.86709999999999998</v>
       </c>
       <c r="G15">
         <v>2.01E-2</v>
@@ -28854,19 +28867,19 @@
         <v>30770</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C18" t="s">
         <v>33</v>
       </c>
       <c r="D18">
-        <v>0.1137</v>
+        <v>0.16800000000000001</v>
       </c>
       <c r="E18">
-        <v>7.3000000000000001E-3</v>
+        <v>2.4899999999999999E-2</v>
       </c>
       <c r="F18">
-        <v>0.96619999999999995</v>
+        <v>0.87</v>
       </c>
       <c r="G18">
         <v>1.9199999999999998E-2</v>
@@ -28927,19 +28940,19 @@
         <v>30700</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C21" t="s">
         <v>33</v>
       </c>
       <c r="D21">
-        <v>0.1328</v>
+        <v>9.7699999999999995E-2</v>
       </c>
       <c r="E21">
-        <v>1.09E-2</v>
+        <v>5.5999999999999999E-3</v>
       </c>
       <c r="F21">
-        <v>0.96589999999999998</v>
+        <v>0.88980000000000004</v>
       </c>
       <c r="G21">
         <v>2.9600000000000001E-2</v>
@@ -28950,19 +28963,19 @@
         <v>21002</v>
       </c>
       <c r="B22" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C22" t="s">
         <v>33</v>
       </c>
       <c r="D22">
-        <v>0.1857</v>
+        <v>0.2049</v>
       </c>
       <c r="E22">
-        <v>1.38E-2</v>
+        <v>1.43E-2</v>
       </c>
       <c r="F22">
-        <v>0.95509999999999995</v>
+        <v>0.89090000000000003</v>
       </c>
       <c r="G22">
         <v>1.3899999999999999E-2</v>
@@ -29065,19 +29078,19 @@
         <v>30680</v>
       </c>
       <c r="B27" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="C27" t="s">
         <v>33</v>
       </c>
       <c r="D27">
-        <v>0.12839999999999999</v>
+        <v>0.1951</v>
       </c>
       <c r="E27">
-        <v>8.2000000000000007E-3</v>
+        <v>7.1000000000000004E-3</v>
       </c>
       <c r="F27">
-        <v>0.94979999999999998</v>
+        <v>0.89290000000000003</v>
       </c>
       <c r="G27">
         <v>2.9499999999999998E-2</v>
@@ -29134,19 +29147,19 @@
         <v>30860</v>
       </c>
       <c r="B30" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="C30" t="s">
         <v>33</v>
       </c>
       <c r="D30">
-        <v>0.2316</v>
+        <v>0.13619999999999999</v>
       </c>
       <c r="E30">
-        <v>8.9999999999999993E-3</v>
+        <v>8.2000000000000007E-3</v>
       </c>
       <c r="F30">
-        <v>0.9466</v>
+        <v>0.89559999999999995</v>
       </c>
       <c r="G30">
         <v>2.69E-2</v>
@@ -29203,19 +29216,19 @@
         <v>30670</v>
       </c>
       <c r="B33" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C33" t="s">
         <v>33</v>
       </c>
       <c r="D33">
-        <v>0.1313</v>
+        <v>0.19689999999999999</v>
       </c>
       <c r="E33">
-        <v>9.5999999999999992E-3</v>
+        <v>6.7000000000000002E-3</v>
       </c>
       <c r="F33">
-        <v>0.94220000000000004</v>
+        <v>0.89629999999999999</v>
       </c>
       <c r="G33">
         <v>3.3599999999999998E-2</v>
@@ -29272,19 +29285,19 @@
         <v>30830</v>
       </c>
       <c r="B36" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C36" t="s">
         <v>33</v>
       </c>
       <c r="D36">
-        <v>0.13400000000000001</v>
+        <v>9.1800000000000007E-2</v>
       </c>
       <c r="E36">
-        <v>5.4999999999999997E-3</v>
+        <v>5.7999999999999996E-3</v>
       </c>
       <c r="F36">
-        <v>0.93730000000000002</v>
+        <v>0.91080000000000005</v>
       </c>
       <c r="G36">
         <v>2.9499999999999998E-2</v>
@@ -29295,19 +29308,19 @@
         <v>23100</v>
       </c>
       <c r="B37" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C37" t="s">
         <v>33</v>
       </c>
       <c r="D37">
-        <v>0.2387</v>
+        <v>0.21829999999999999</v>
       </c>
       <c r="E37">
-        <v>8.6E-3</v>
+        <v>7.1999999999999998E-3</v>
       </c>
       <c r="F37">
-        <v>0.9365</v>
+        <v>0.91349999999999998</v>
       </c>
       <c r="G37">
         <v>1.44E-2</v>
@@ -29410,19 +29423,19 @@
         <v>20151</v>
       </c>
       <c r="B42" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C42" t="s">
         <v>33</v>
       </c>
       <c r="D42">
-        <v>0.23169999999999999</v>
+        <v>0.1278</v>
       </c>
       <c r="E42">
-        <v>8.9999999999999993E-3</v>
+        <v>5.4000000000000003E-3</v>
       </c>
       <c r="F42">
-        <v>0.93269999999999997</v>
+        <v>0.92410000000000003</v>
       </c>
       <c r="G42">
         <v>2.0500000000000001E-2</v>
@@ -29548,19 +29561,19 @@
         <v>30880</v>
       </c>
       <c r="B48" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C48" t="s">
         <v>33</v>
       </c>
       <c r="D48">
-        <v>0.1278</v>
+        <v>0.23169999999999999</v>
       </c>
       <c r="E48">
-        <v>5.4000000000000003E-3</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="F48">
-        <v>0.92410000000000003</v>
+        <v>0.93269999999999997</v>
       </c>
       <c r="G48">
         <v>3.1099999999999999E-2</v>
@@ -29571,19 +29584,19 @@
         <v>23125</v>
       </c>
       <c r="B49" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C49" t="s">
         <v>33</v>
       </c>
       <c r="D49">
-        <v>0.21829999999999999</v>
+        <v>0.2387</v>
       </c>
       <c r="E49">
-        <v>7.1999999999999998E-3</v>
+        <v>8.6E-3</v>
       </c>
       <c r="F49">
-        <v>0.91349999999999998</v>
+        <v>0.9365</v>
       </c>
       <c r="G49">
         <v>1.44E-2</v>
@@ -29640,19 +29653,19 @@
         <v>23121</v>
       </c>
       <c r="B52" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C52" t="s">
         <v>33</v>
       </c>
       <c r="D52">
-        <v>9.1800000000000007E-2</v>
+        <v>0.13400000000000001</v>
       </c>
       <c r="E52">
-        <v>5.7999999999999996E-3</v>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="F52">
-        <v>0.91080000000000005</v>
+        <v>0.93730000000000002</v>
       </c>
       <c r="G52">
         <v>1.38E-2</v>
@@ -29755,19 +29768,19 @@
         <v>30210</v>
       </c>
       <c r="B57" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C57" t="s">
         <v>33</v>
       </c>
       <c r="D57">
-        <v>0.19689999999999999</v>
+        <v>0.1313</v>
       </c>
       <c r="E57">
-        <v>6.7000000000000002E-3</v>
+        <v>9.5999999999999992E-3</v>
       </c>
       <c r="F57">
-        <v>0.89629999999999999</v>
+        <v>0.94220000000000004</v>
       </c>
       <c r="G57">
         <v>2.4899999999999999E-2</v>
@@ -29824,19 +29837,19 @@
         <v>30180</v>
       </c>
       <c r="B60" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C60" t="s">
         <v>33</v>
       </c>
       <c r="D60">
-        <v>0.13619999999999999</v>
+        <v>0.2316</v>
       </c>
       <c r="E60">
-        <v>8.2000000000000007E-3</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="F60">
-        <v>0.89559999999999995</v>
+        <v>0.9466</v>
       </c>
       <c r="G60">
         <v>2.2499999999999999E-2</v>
@@ -29893,19 +29906,19 @@
         <v>48</v>
       </c>
       <c r="B63" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C63" t="s">
         <v>33</v>
       </c>
       <c r="D63">
-        <v>0.1951</v>
+        <v>0.12839999999999999</v>
       </c>
       <c r="E63">
-        <v>7.1000000000000004E-3</v>
+        <v>8.2000000000000007E-3</v>
       </c>
       <c r="F63">
-        <v>0.89290000000000003</v>
+        <v>0.94979999999999998</v>
       </c>
       <c r="G63">
         <v>1.7000000000000001E-2</v>
@@ -29916,19 +29929,19 @@
         <v>49</v>
       </c>
       <c r="B64" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C64" t="s">
         <v>33</v>
       </c>
       <c r="D64">
-        <v>0.2049</v>
+        <v>0.1857</v>
       </c>
       <c r="E64">
-        <v>1.43E-2</v>
+        <v>1.38E-2</v>
       </c>
       <c r="F64">
-        <v>0.89090000000000003</v>
+        <v>0.95509999999999995</v>
       </c>
       <c r="G64">
         <v>1.6400000000000001E-2</v>
@@ -29985,19 +29998,19 @@
         <v>0</v>
       </c>
       <c r="B67" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C67" t="s">
         <v>33</v>
       </c>
       <c r="D67">
-        <v>9.7699999999999995E-2</v>
+        <v>0.1328</v>
       </c>
       <c r="E67">
-        <v>5.5999999999999999E-3</v>
+        <v>1.09E-2</v>
       </c>
       <c r="F67">
-        <v>0.88980000000000004</v>
+        <v>0.96589999999999998</v>
       </c>
       <c r="G67">
         <v>2.52E-2</v>
@@ -30054,19 +30067,19 @@
         <v>0</v>
       </c>
       <c r="B70" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="C70" t="s">
         <v>33</v>
       </c>
       <c r="D70">
-        <v>0.16800000000000001</v>
+        <v>0.1137</v>
       </c>
       <c r="E70">
-        <v>2.4899999999999999E-2</v>
+        <v>7.3000000000000001E-3</v>
       </c>
       <c r="F70">
-        <v>0.87</v>
+        <v>0.96619999999999995</v>
       </c>
       <c r="G70">
         <v>2.69E-2</v>
@@ -30123,19 +30136,19 @@
         <v>4079</v>
       </c>
       <c r="B73" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C73" t="s">
         <v>33</v>
       </c>
       <c r="D73">
-        <v>0.157</v>
+        <v>0.1065</v>
       </c>
       <c r="E73">
-        <v>2.69E-2</v>
+        <v>1.11E-2</v>
       </c>
       <c r="F73">
-        <v>0.86709999999999998</v>
+        <v>0.96630000000000005</v>
       </c>
       <c r="G73">
         <v>2.7400000000000001E-2</v>
@@ -30192,19 +30205,19 @@
         <v>4080</v>
       </c>
       <c r="B76" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="C76" t="s">
         <v>33</v>
       </c>
       <c r="D76">
-        <v>0.158</v>
+        <v>0.42020000000000002</v>
       </c>
       <c r="E76">
-        <v>5.3E-3</v>
+        <v>1.7399999999999999E-2</v>
       </c>
       <c r="F76">
-        <v>0.75170000000000003</v>
+        <v>0.97230000000000005</v>
       </c>
       <c r="G76">
         <v>2.53E-2</v>
@@ -30261,19 +30274,19 @@
         <v>23479</v>
       </c>
       <c r="B79" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C79" t="s">
         <v>33</v>
       </c>
       <c r="D79">
-        <v>0.12820000000000001</v>
+        <v>0.1973</v>
       </c>
       <c r="E79">
-        <v>7.1999999999999998E-3</v>
+        <v>7.7000000000000002E-3</v>
       </c>
       <c r="F79">
-        <v>0.63219999999999998</v>
+        <v>0.9728</v>
       </c>
       <c r="G79">
         <v>3.1E-2</v>
@@ -30330,19 +30343,19 @@
         <v>102</v>
       </c>
       <c r="B82" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C82" t="s">
         <v>33</v>
       </c>
       <c r="D82">
-        <v>8.5000000000000006E-2</v>
+        <v>0.10630000000000001</v>
       </c>
       <c r="E82">
-        <v>1.1299999999999999E-2</v>
+        <v>6.8999999999999999E-3</v>
       </c>
       <c r="F82">
-        <v>1.12E-2</v>
+        <v>0.98</v>
       </c>
       <c r="G82">
         <v>2.5999999999999999E-2</v>
@@ -30401,8 +30414,8 @@
         <filter val="both_sex"/>
       </filters>
     </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:F84">
-      <sortCondition descending="1" ref="F3:F84"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B6:F82">
+      <sortCondition ref="F3:F84"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -30417,7 +30430,7 @@
       <pane xSplit="9" ySplit="3" topLeftCell="J4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4:A30"/>
+      <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -30429,6 +30442,7 @@
     <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.54296875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.6328125" customWidth="1"/>
+    <col min="9" max="9" width="10.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -30456,7 +30470,9 @@
       <c r="H3" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="I3" s="1"/>
+      <c r="I3" s="1" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -30471,6 +30487,9 @@
       <c r="D4">
         <v>1</v>
       </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
       <c r="F4">
         <v>1</v>
       </c>
@@ -30478,6 +30497,9 @@
         <v>1</v>
       </c>
       <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
         <v>1</v>
       </c>
     </row>
@@ -30494,6 +30516,9 @@
       <c r="D5">
         <v>1</v>
       </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
       <c r="F5">
         <v>1</v>
       </c>
@@ -30501,6 +30526,9 @@
         <v>1</v>
       </c>
       <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
         <v>1</v>
       </c>
     </row>
@@ -30517,10 +30545,16 @@
       <c r="D6">
         <v>1</v>
       </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="I6">
         <v>1</v>
       </c>
     </row>
@@ -30537,10 +30571,16 @@
       <c r="D7">
         <v>1</v>
       </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="I7">
         <v>1</v>
       </c>
     </row>
@@ -30557,10 +30597,16 @@
       <c r="D8">
         <v>1</v>
       </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="I8">
         <v>1</v>
       </c>
     </row>
@@ -30577,10 +30623,16 @@
       <c r="D9">
         <v>1</v>
       </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
       <c r="F9">
         <v>1</v>
       </c>
       <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="I9">
         <v>1</v>
       </c>
     </row>
@@ -30597,6 +30649,9 @@
       <c r="D10">
         <v>1</v>
       </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
       <c r="F10">
         <v>1</v>
       </c>
@@ -30604,6 +30659,9 @@
         <v>1</v>
       </c>
       <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
         <v>1</v>
       </c>
     </row>
@@ -30620,10 +30678,16 @@
       <c r="D11">
         <v>1</v>
       </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
       <c r="F11">
         <v>1</v>
       </c>
       <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="I11">
         <v>1</v>
       </c>
     </row>
@@ -30640,10 +30704,16 @@
       <c r="D12">
         <v>1</v>
       </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
       <c r="F12">
         <v>1</v>
       </c>
       <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="I12">
         <v>1</v>
       </c>
     </row>
@@ -30660,10 +30730,16 @@
       <c r="D13">
         <v>1</v>
       </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
       <c r="F13">
         <v>1</v>
       </c>
       <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="I13">
         <v>1</v>
       </c>
     </row>
@@ -30680,10 +30756,16 @@
       <c r="D14">
         <v>1</v>
       </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
       <c r="F14">
         <v>1</v>
       </c>
       <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="I14">
         <v>1</v>
       </c>
     </row>
@@ -30700,6 +30782,9 @@
       <c r="D15">
         <v>1</v>
       </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
       <c r="F15">
         <v>1</v>
       </c>
@@ -30707,6 +30792,9 @@
         <v>1</v>
       </c>
       <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
         <v>1</v>
       </c>
     </row>
@@ -30723,14 +30811,20 @@
       <c r="D16">
         <v>1</v>
       </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
       <c r="F16">
         <v>1</v>
       </c>
       <c r="G16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="28" t="s">
         <v>19</v>
       </c>
@@ -30743,14 +30837,20 @@
       <c r="D17">
         <v>1</v>
       </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
       <c r="F17">
         <v>1</v>
       </c>
       <c r="G17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="28" t="s">
         <v>20</v>
       </c>
@@ -30763,6 +30863,9 @@
       <c r="D18">
         <v>1</v>
       </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
       <c r="F18">
         <v>1</v>
       </c>
@@ -30772,8 +30875,11 @@
       <c r="H18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="28" t="s">
         <v>21</v>
       </c>
@@ -30786,14 +30892,20 @@
       <c r="D19">
         <v>1</v>
       </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
       <c r="F19">
         <v>1</v>
       </c>
       <c r="G19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="28" t="s">
         <v>22</v>
       </c>
@@ -30806,14 +30918,20 @@
       <c r="D20">
         <v>1</v>
       </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
       <c r="F20">
         <v>1</v>
       </c>
       <c r="G20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="28" t="s">
         <v>23</v>
       </c>
@@ -30826,14 +30944,20 @@
       <c r="D21">
         <v>1</v>
       </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
       <c r="F21">
         <v>1</v>
       </c>
       <c r="G21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="28" t="s">
         <v>24</v>
       </c>
@@ -30846,14 +30970,20 @@
       <c r="D22">
         <v>1</v>
       </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
       <c r="F22">
         <v>1</v>
       </c>
       <c r="G22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="28" t="s">
         <v>25</v>
       </c>
@@ -30866,14 +30996,20 @@
       <c r="D23">
         <v>1</v>
       </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
       <c r="F23">
         <v>1</v>
       </c>
       <c r="G23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="28" t="s">
         <v>26</v>
       </c>
@@ -30886,14 +31022,20 @@
       <c r="D24">
         <v>1</v>
       </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
       <c r="F24">
         <v>1</v>
       </c>
       <c r="G24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="28" t="s">
         <v>27</v>
       </c>
@@ -30906,14 +31048,20 @@
       <c r="D25">
         <v>1</v>
       </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
       <c r="F25">
         <v>1</v>
       </c>
       <c r="G25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="28" t="s">
         <v>28</v>
       </c>
@@ -30926,34 +31074,43 @@
       <c r="D26">
         <v>1</v>
       </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
       <c r="F26">
         <v>1</v>
       </c>
       <c r="G26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="I26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="28" t="s">
         <v>29</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
       <c r="D27">
         <v>1</v>
       </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
       <c r="F27">
         <v>1</v>
       </c>
       <c r="G27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="I27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="28" t="s">
         <v>30</v>
       </c>
@@ -30966,14 +31123,20 @@
       <c r="D28">
         <v>1</v>
       </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
       <c r="F28">
         <v>1</v>
       </c>
       <c r="G28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="28" t="s">
         <v>31</v>
       </c>
@@ -30986,14 +31149,20 @@
       <c r="D29">
         <v>1</v>
       </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
       <c r="F29">
         <v>1</v>
       </c>
       <c r="G29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="34" t="s">
         <v>32</v>
       </c>
@@ -31006,7 +31175,9 @@
       <c r="D30" s="35">
         <v>1</v>
       </c>
-      <c r="E30" s="35"/>
+      <c r="E30" s="35">
+        <v>1</v>
+      </c>
       <c r="F30" s="35">
         <v>1</v>
       </c>
@@ -31014,13 +31185,16 @@
         <v>1</v>
       </c>
       <c r="H30" s="35"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I30" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="28" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="29" t="s">
         <v>64</v>
       </c>
@@ -32509,24 +32683,24 @@
     <row r="2" spans="1:14" ht="26" x14ac:dyDescent="0.6">
       <c r="A2" s="6"/>
       <c r="B2" s="7"/>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="36" t="s">
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="36" t="s">
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
     </row>
     <row r="3" spans="1:14" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="15" t="s">
@@ -37850,24 +38024,24 @@
     <row r="2" spans="1:14" ht="26" x14ac:dyDescent="0.6">
       <c r="A2" s="6"/>
       <c r="B2" s="7"/>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="36" t="s">
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="36" t="s">
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
     </row>
     <row r="3" spans="1:14" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="15" t="s">
@@ -42381,24 +42555,24 @@
     <row r="2" spans="1:14" ht="26" x14ac:dyDescent="0.6">
       <c r="A2" s="6"/>
       <c r="B2" s="7"/>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="36" t="s">
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="36" t="s">
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
     </row>
     <row r="3" spans="1:14" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="15" t="s">
@@ -46858,24 +47032,24 @@
     <row r="2" spans="1:14" ht="26" x14ac:dyDescent="0.6">
       <c r="A2" s="6"/>
       <c r="B2" s="7"/>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="36" t="s">
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="36" t="s">
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
     </row>
     <row r="3" spans="1:14" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="15" t="s">

</xml_diff>